<commit_message>
design now includes USB charger
</commit_message>
<xml_diff>
--- a/DressCode BOM.xlsx
+++ b/DressCode BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -24,9 +24,6 @@
     <t>2.2k, 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C3, C4 </t>
-  </si>
-  <si>
     <t>10u, 0805</t>
   </si>
   <si>
@@ -39,15 +36,9 @@
     <t>U3</t>
   </si>
   <si>
-    <t>MCP6G02 (SGA)</t>
-  </si>
-  <si>
     <t>U1, U2</t>
   </si>
   <si>
-    <t>MCP6S21 (PGA)</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -78,16 +69,43 @@
     <t>Only one microphone should be populated, M1 or M2</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7</t>
-  </si>
-  <si>
-    <t>R8, R9, R10</t>
-  </si>
-  <si>
     <t>100R, 0805</t>
   </si>
   <si>
     <t>PIC24FV16KA304-I/PT</t>
+  </si>
+  <si>
+    <t>C1, C3, C4, C5, C6</t>
+  </si>
+  <si>
+    <t>R9, R10, R11</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8</t>
+  </si>
+  <si>
+    <t>USB1</t>
+  </si>
+  <si>
+    <t>Micro USB socket</t>
+  </si>
+  <si>
+    <t>JST1</t>
+  </si>
+  <si>
+    <t>JST battery connector</t>
+  </si>
+  <si>
+    <t>MCP73832T-2ACI/OT (battery charger)</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>MCP6G02-E/SN (SGA)</t>
+  </si>
+  <si>
+    <t>MCP6S21-I/SN (PGA)</t>
   </si>
 </sst>
 </file>
@@ -470,16 +488,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="10.85546875" style="6" customWidth="1"/>
   </cols>
@@ -489,42 +507,42 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F3" s="6">
         <f>D3*E3</f>
-        <v>0.105</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -533,34 +551,34 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" ref="F4:F11" si="0">D4*E4</f>
+        <f t="shared" ref="F4:F14" si="0">D4*E4</f>
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" s="6">
         <v>0.02</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -575,10 +593,10 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -593,10 +611,10 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -611,10 +629,10 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -629,10 +647,10 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -647,10 +665,10 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -664,40 +682,97 @@
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="E13" s="8" t="s">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="E16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="6">
+        <f>SUM(F3:F15)</f>
+        <v>6.3339999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
         <v>16</v>
-      </c>
-      <c r="F13" s="6">
-        <f>SUM(F3:F12)</f>
-        <v>4.891</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" display="PIC24FV32KA304-I/PT"/>
-    <hyperlink ref="C8" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId2" display="MCP6S21 (PGA)"/>
+    <hyperlink ref="C7" r:id="rId3" display="MCP6G02 (SGA)"/>
     <hyperlink ref="C6" r:id="rId4"/>
     <hyperlink ref="C5" r:id="rId5"/>
     <hyperlink ref="C9" r:id="rId6"/>
     <hyperlink ref="C3" r:id="rId7"/>
     <hyperlink ref="C10" r:id="rId8"/>
     <hyperlink ref="C4" r:id="rId9"/>
+    <hyperlink ref="C13" r:id="rId10"/>
+    <hyperlink ref="C14" r:id="rId11"/>
+    <hyperlink ref="C12" r:id="rId12" display="MCP73832T-2ACI/OT"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add C2 to BOM and USB rework photo
</commit_message>
<xml_diff>
--- a/DressCode BOM.xlsx
+++ b/DressCode BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Slide switch</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>10n, 0805</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,7 +563,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" ref="F4:F15" si="0">D4*E4</f>
+        <f t="shared" ref="F4:F16" si="0">D4*E4</f>
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
@@ -581,79 +587,79 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6">
-        <v>2.7E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
-        <v>8.1000000000000003E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="6">
-        <v>0.314</v>
+        <v>2.7E-2</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>0.314</v>
+        <v>8.1000000000000003E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>0.68600000000000005</v>
+        <v>0.314</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="0"/>
-        <v>1.3720000000000001</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="6">
-        <v>0.46400000000000002</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="0"/>
-        <v>0.46400000000000002</v>
+        <v>1.3720000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>8</v>
@@ -662,142 +668,161 @@
         <v>1</v>
       </c>
       <c r="E10" s="6">
-        <v>0.56399999999999995</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>0.56399999999999995</v>
+        <v>0.46400000000000002</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="6">
-        <v>1.91</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>1.91</v>
+        <v>0.56399999999999995</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="6">
-        <v>0.38</v>
+        <v>1.91</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
-        <v>0.38</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="6">
-        <v>0.51800000000000002</v>
+        <v>0.38</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>0.51800000000000002</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="6">
-        <v>0.49</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>0.49</v>
+        <v>0.51800000000000002</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
         <v>0.62</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F16" s="6">
         <f t="shared" si="0"/>
         <v>0.62</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
     <row r="17" spans="2:6">
-      <c r="E17" s="8" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="E18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="6">
-        <f>SUM(F3:F16)</f>
-        <v>6.9539999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" t="s">
+      <c r="F18" s="6">
+        <f>SUM(F3:F17)</f>
+        <v>6.9740000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="PIC24FV32KA304-I/PT"/>
-    <hyperlink ref="C8" r:id="rId2" display="MCP6S21 (PGA)"/>
-    <hyperlink ref="C7" r:id="rId3" display="MCP6G02 (SGA)"/>
-    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C12" r:id="rId1" display="PIC24FV32KA304-I/PT"/>
+    <hyperlink ref="C9" r:id="rId2" display="MCP6S21 (PGA)"/>
+    <hyperlink ref="C8" r:id="rId3" display="MCP6G02 (SGA)"/>
+    <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C5" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C10" r:id="rId6"/>
     <hyperlink ref="C3" r:id="rId7"/>
-    <hyperlink ref="C10" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="C4" r:id="rId9"/>
-    <hyperlink ref="C13" r:id="rId10"/>
-    <hyperlink ref="C14" r:id="rId11"/>
-    <hyperlink ref="C12" r:id="rId12" display="MCP73832T-2ACI/OT"/>
-    <hyperlink ref="C15" r:id="rId13"/>
+    <hyperlink ref="C14" r:id="rId10"/>
+    <hyperlink ref="C15" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12" display="MCP73832T-2ACI/OT"/>
+    <hyperlink ref="C16" r:id="rId13"/>
+    <hyperlink ref="C6" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Correct link to 10uF capacitor in BOM
</commit_message>
<xml_diff>
--- a/DressCode BOM.xlsx
+++ b/DressCode BOM.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -578,11 +578,11 @@
         <v>5</v>
       </c>
       <c r="E5" s="6">
-        <v>0.02</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="6" spans="2:6">
@@ -796,7 +796,7 @@
       </c>
       <c r="F18" s="6">
         <f>SUM(F3:F17)</f>
-        <v>6.9740000000000002</v>
+        <v>7.2439999999999998</v>
       </c>
     </row>
     <row r="20" spans="2:6">

</xml_diff>